<commit_message>
one dashboard down, a couple more to go
</commit_message>
<xml_diff>
--- a/Data/H1B_USCIS_15_20.xlsx
+++ b/Data/H1B_USCIS_15_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thewillisgroup-my.sharepoint.com/personal/isoto_talentpath_com/Documents/H1B_and_Technology/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{2A1B2CC8-54F1-45BE-9534-B035BB568C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F216782B-4D75-4EF3-AA48-1989BAB2429F}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{2A1B2CC8-54F1-45BE-9534-B035BB568C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3FEA2D2-DDDB-4AFC-A28A-522050E2EEEE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{229B963B-C8B3-4D64-A9B2-07794C00DFB1}"/>
+    <workbookView xWindow="28680" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{229B963B-C8B3-4D64-A9B2-07794C00DFB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,127 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>OCT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NOV</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>DEC</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>JAN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>FEB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>MAR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>APR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>MAY</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>JUN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>JUL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>AUG</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>SEP</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
   <si>
     <r>
       <rPr>
@@ -289,40 +169,40 @@
     </r>
   </si>
   <si>
-    <t>OCT</t>
+    <t>April</t>
   </si>
   <si>
-    <t>NOV</t>
+    <t>August</t>
   </si>
   <si>
-    <t>DEC</t>
+    <t>December</t>
   </si>
   <si>
-    <t>JAN</t>
+    <t>February</t>
   </si>
   <si>
-    <t>FEB</t>
+    <t>January</t>
   </si>
   <si>
-    <t>MAR</t>
+    <t>July</t>
   </si>
   <si>
-    <t>APR</t>
+    <t>June</t>
   </si>
   <si>
-    <t>MAY</t>
+    <t>March</t>
   </si>
   <si>
-    <t>JUN</t>
+    <t>May</t>
   </si>
   <si>
-    <t>JUL</t>
+    <t>November</t>
   </si>
   <si>
-    <t>AUG</t>
+    <t>October</t>
   </si>
   <si>
-    <t>SEP</t>
+    <t>September</t>
   </si>
 </sst>
 </file>
@@ -377,9 +257,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC2018C-689B-4FAA-A8D7-89D1F2A0013A}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,45 +629,45 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2015</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C2">
         <v>20252</v>
@@ -820,8 +701,8 @@
       <c r="A3">
         <v>2015</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C3">
         <v>16071</v>
@@ -855,8 +736,8 @@
       <c r="A4">
         <v>2015</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C4">
         <v>15709</v>
@@ -890,8 +771,8 @@
       <c r="A5">
         <v>2015</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
         <v>13638</v>
@@ -925,8 +806,8 @@
       <c r="A6">
         <v>2015</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C6">
         <v>14583</v>
@@ -960,8 +841,8 @@
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C7">
         <v>17917</v>
@@ -995,8 +876,8 @@
       <c r="A8">
         <v>2015</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C8">
         <v>120225</v>
@@ -1030,8 +911,8 @@
       <c r="A9">
         <v>2015</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C9">
         <v>25667</v>
@@ -1065,8 +946,8 @@
       <c r="A10">
         <v>2015</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C10">
         <v>30541</v>
@@ -1100,8 +981,8 @@
       <c r="A11">
         <v>2015</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C11">
         <v>31995</v>
@@ -1135,8 +1016,8 @@
       <c r="A12">
         <v>2015</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C12">
         <v>31448</v>
@@ -1170,8 +1051,8 @@
       <c r="A13">
         <v>2015</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C13">
         <v>30117</v>
@@ -1205,8 +1086,8 @@
       <c r="A14">
         <v>2016</v>
       </c>
-      <c r="B14" t="s">
-        <v>0</v>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C14">
         <v>24324</v>
@@ -1240,8 +1121,8 @@
       <c r="A15">
         <v>2016</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C15">
         <v>19598</v>
@@ -1275,8 +1156,8 @@
       <c r="A16">
         <v>2016</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C16">
         <v>20817</v>
@@ -1310,8 +1191,8 @@
       <c r="A17">
         <v>2016</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C17">
         <v>19768</v>
@@ -1345,8 +1226,8 @@
       <c r="A18">
         <v>2016</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C18">
         <v>21867</v>
@@ -1380,8 +1261,8 @@
       <c r="A19">
         <v>2016</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C19">
         <v>25120</v>
@@ -1415,8 +1296,8 @@
       <c r="A20">
         <v>2016</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C20">
         <v>122912</v>
@@ -1450,8 +1331,8 @@
       <c r="A21">
         <v>2016</v>
       </c>
-      <c r="B21" t="s">
-        <v>7</v>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C21">
         <v>31824</v>
@@ -1485,8 +1366,8 @@
       <c r="A22">
         <v>2016</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C22">
         <v>31036</v>
@@ -1520,8 +1401,8 @@
       <c r="A23">
         <v>2016</v>
       </c>
-      <c r="B23" t="s">
-        <v>9</v>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C23">
         <v>26648</v>
@@ -1555,8 +1436,8 @@
       <c r="A24">
         <v>2016</v>
       </c>
-      <c r="B24" t="s">
-        <v>10</v>
+      <c r="B24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C24">
         <v>28732</v>
@@ -1590,8 +1471,8 @@
       <c r="A25">
         <v>2016</v>
       </c>
-      <c r="B25" t="s">
-        <v>11</v>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C25">
         <v>26157</v>
@@ -1625,8 +1506,8 @@
       <c r="A26">
         <v>2017</v>
       </c>
-      <c r="B26" t="s">
-        <v>0</v>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C26">
         <v>22625</v>
@@ -1660,8 +1541,8 @@
       <c r="A27">
         <v>2017</v>
       </c>
-      <c r="B27" t="s">
-        <v>1</v>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C27">
         <v>20699</v>
@@ -1695,8 +1576,8 @@
       <c r="A28">
         <v>2017</v>
       </c>
-      <c r="B28" t="s">
-        <v>2</v>
+      <c r="B28" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C28">
         <v>21684</v>
@@ -1730,8 +1611,8 @@
       <c r="A29">
         <v>2017</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
+      <c r="B29" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C29">
         <v>19999</v>
@@ -1765,8 +1646,8 @@
       <c r="A30">
         <v>2017</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
+      <c r="B30" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C30">
         <v>21685</v>
@@ -1800,8 +1681,8 @@
       <c r="A31">
         <v>2017</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C31">
         <v>55381</v>
@@ -1835,8 +1716,8 @@
       <c r="A32">
         <v>2017</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
+      <c r="B32" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C32">
         <v>115095</v>
@@ -1870,8 +1751,8 @@
       <c r="A33">
         <v>2017</v>
       </c>
-      <c r="B33" t="s">
-        <v>7</v>
+      <c r="B33" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C33">
         <v>27061</v>
@@ -1905,8 +1786,8 @@
       <c r="A34">
         <v>2017</v>
       </c>
-      <c r="B34" t="s">
-        <v>8</v>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C34">
         <v>27162</v>
@@ -1940,8 +1821,8 @@
       <c r="A35">
         <v>2017</v>
       </c>
-      <c r="B35" t="s">
-        <v>9</v>
+      <c r="B35" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C35">
         <v>23425</v>
@@ -1975,8 +1856,8 @@
       <c r="A36">
         <v>2017</v>
       </c>
-      <c r="B36" t="s">
-        <v>10</v>
+      <c r="B36" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C36">
         <v>25870</v>
@@ -2010,8 +1891,8 @@
       <c r="A37">
         <v>2017</v>
       </c>
-      <c r="B37" t="s">
-        <v>11</v>
+      <c r="B37" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C37">
         <v>22469</v>
@@ -2045,8 +1926,8 @@
       <c r="A38">
         <v>2018</v>
       </c>
-      <c r="B38" t="s">
-        <v>0</v>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C38">
         <v>21890</v>
@@ -2080,8 +1961,8 @@
       <c r="A39">
         <v>2018</v>
       </c>
-      <c r="B39" t="s">
-        <v>1</v>
+      <c r="B39" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C39">
         <v>20361</v>
@@ -2115,8 +1996,8 @@
       <c r="A40">
         <v>2018</v>
       </c>
-      <c r="B40" t="s">
-        <v>2</v>
+      <c r="B40" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C40">
         <v>20067</v>
@@ -2150,8 +2031,8 @@
       <c r="A41">
         <v>2018</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
+      <c r="B41" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C41">
         <v>20965</v>
@@ -2185,8 +2066,8 @@
       <c r="A42">
         <v>2018</v>
       </c>
-      <c r="B42" t="s">
-        <v>4</v>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C42">
         <v>22939</v>
@@ -2220,8 +2101,8 @@
       <c r="A43">
         <v>2018</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
+      <c r="B43" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C43">
         <v>25696</v>
@@ -2255,8 +2136,8 @@
       <c r="A44">
         <v>2018</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
+      <c r="B44" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C44">
         <v>139538</v>
@@ -2290,8 +2171,8 @@
       <c r="A45">
         <v>2018</v>
       </c>
-      <c r="B45" t="s">
-        <v>7</v>
+      <c r="B45" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C45">
         <v>33032</v>
@@ -2325,8 +2206,8 @@
       <c r="A46">
         <v>2018</v>
       </c>
-      <c r="B46" t="s">
-        <v>8</v>
+      <c r="B46" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C46">
         <v>29837</v>
@@ -2360,8 +2241,8 @@
       <c r="A47">
         <v>2018</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
+      <c r="B47" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C47">
         <v>27721</v>
@@ -2395,8 +2276,8 @@
       <c r="A48">
         <v>2018</v>
       </c>
-      <c r="B48" t="s">
-        <v>10</v>
+      <c r="B48" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C48">
         <v>29467</v>
@@ -2430,8 +2311,8 @@
       <c r="A49">
         <v>2018</v>
       </c>
-      <c r="B49" t="s">
-        <v>11</v>
+      <c r="B49" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C49">
         <v>27277</v>
@@ -2465,8 +2346,8 @@
       <c r="A50">
         <v>2019</v>
       </c>
-      <c r="B50" t="s">
-        <v>23</v>
+      <c r="B50" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C50">
         <v>19819</v>
@@ -2500,8 +2381,8 @@
       <c r="A51">
         <v>2019</v>
       </c>
-      <c r="B51" t="s">
-        <v>24</v>
+      <c r="B51" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C51">
         <v>19640</v>
@@ -2535,8 +2416,8 @@
       <c r="A52">
         <v>2019</v>
       </c>
-      <c r="B52" t="s">
-        <v>25</v>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C52">
         <v>20839</v>
@@ -2570,8 +2451,8 @@
       <c r="A53">
         <v>2019</v>
       </c>
-      <c r="B53" t="s">
-        <v>26</v>
+      <c r="B53" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C53">
         <v>20106</v>
@@ -2605,8 +2486,8 @@
       <c r="A54">
         <v>2019</v>
       </c>
-      <c r="B54" t="s">
-        <v>27</v>
+      <c r="B54" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C54">
         <v>21397</v>
@@ -2640,8 +2521,8 @@
       <c r="A55">
         <v>2019</v>
       </c>
-      <c r="B55" t="s">
-        <v>28</v>
+      <c r="B55" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C55">
         <v>25796</v>
@@ -2675,8 +2556,8 @@
       <c r="A56">
         <v>2019</v>
       </c>
-      <c r="B56" t="s">
-        <v>29</v>
+      <c r="B56" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C56">
         <v>140247</v>
@@ -2710,8 +2591,8 @@
       <c r="A57">
         <v>2019</v>
       </c>
-      <c r="B57" t="s">
-        <v>30</v>
+      <c r="B57" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C57">
         <v>35196</v>
@@ -2745,8 +2626,8 @@
       <c r="A58">
         <v>2019</v>
       </c>
-      <c r="B58" t="s">
-        <v>31</v>
+      <c r="B58" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C58">
         <v>31305</v>
@@ -2780,8 +2661,8 @@
       <c r="A59">
         <v>2019</v>
       </c>
-      <c r="B59" t="s">
-        <v>32</v>
+      <c r="B59" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C59">
         <v>31096</v>
@@ -2815,8 +2696,8 @@
       <c r="A60">
         <v>2019</v>
       </c>
-      <c r="B60" t="s">
-        <v>33</v>
+      <c r="B60" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C60">
         <v>29555</v>
@@ -2850,8 +2731,8 @@
       <c r="A61">
         <v>2019</v>
       </c>
-      <c r="B61" t="s">
-        <v>34</v>
+      <c r="B61" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C61">
         <v>25636</v>
@@ -2885,8 +2766,8 @@
       <c r="A62">
         <v>2020</v>
       </c>
-      <c r="B62" t="s">
-        <v>23</v>
+      <c r="B62" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C62">
         <v>26331</v>
@@ -2920,8 +2801,8 @@
       <c r="A63">
         <v>2020</v>
       </c>
-      <c r="B63" t="s">
-        <v>24</v>
+      <c r="B63" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C63">
         <v>25699</v>
@@ -2955,8 +2836,8 @@
       <c r="A64">
         <v>2020</v>
       </c>
-      <c r="B64" t="s">
-        <v>25</v>
+      <c r="B64" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C64">
         <v>25869</v>
@@ -3001,15 +2882,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008284AD765DC00468CDB6C7FC9C8B3B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e256d79a34532ba5ccb4e22275557b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b5fb8014-055b-46b0-a878-751513a12609" xmlns:ns4="3bbb715c-848a-4971-9aa6-2621d55eea22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a662233147e2dcbf0fb7f68d699675a3" ns3:_="" ns4:_="">
     <xsd:import namespace="b5fb8014-055b-46b0-a878-751513a12609"/>
@@ -3226,6 +3098,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF09305A-0FC3-407D-BDF6-291F2D957F50}">
   <ds:schemaRefs>
@@ -3236,14 +3117,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FEA0F29-200D-4C1E-AA13-B1954580F465}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8C5617-F7D0-4B22-B294-4F887D09A094}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3260,4 +3133,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FEA0F29-200D-4C1E-AA13-B1954580F465}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>